<commit_message>
New Changes including API and E2E Testing
</commit_message>
<xml_diff>
--- a/testData/testDataDEV.xlsx
+++ b/testData/testDataDEV.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\eclipse-workspace\DemoProject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F960DC6F-DF32-4680-9F40-77A8EC6AFA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A885454F-FB18-4F46-A468-F89BB7874C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchProduct" sheetId="2" r:id="rId2"/>
+    <sheet name="CheckOut" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Username</t>
   </si>
@@ -40,6 +42,30 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bike Light</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Santa</t>
+  </si>
+  <si>
+    <t>700156</t>
   </si>
 </sst>
 </file>
@@ -75,11 +101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,7 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -400,4 +427,71 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D757F9B0-4589-4643-A6FE-6184DF9D7A58}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BC2307-1781-446F-80B5-C67560EC327B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
third commit including jenkins
</commit_message>
<xml_diff>
--- a/testData/testDataDEV.xlsx
+++ b/testData/testDataDEV.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\eclipse-workspace\DemoProject\testData\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Username</t>
   </si>
@@ -66,12 +66,55 @@
   </si>
   <si>
     <t>700156</t>
+  </si>
+  <si>
+    <t>Updated Value</t>
+  </si>
+  <si>
+    <t>New Value</t>
+  </si>
+  <si>
+    <t>Logged in asstandard_user</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241225_163609</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241225_172740</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241225_172834</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241225_174206</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241225_190127</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241225_200712</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241225_204903</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241225_211614</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241226_055522</t>
+  </si>
+  <si>
+    <t>Logged in as standard_user_20241227_010034</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -395,15 +438,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="30.54296875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.453125"/>
+    <col min="2" max="2" customWidth="true" width="30.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -414,9 +457,12 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">

</xml_diff>